<commit_message>
updated temp data and size data
</commit_message>
<xml_diff>
--- a/data/temperature.xlsx
+++ b/data/temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/vims-resazurin/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB367F43-4442-BD4B-8E8F-6BE551A35F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546BD29D-3768-0946-9EAF-693DA96B83A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="10000" windowHeight="16940" xr2:uid="{AD456542-BC20-0241-8701-D925B25ABE5D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -144,6 +144,42 @@
   </si>
   <si>
     <t>plate31</t>
+  </si>
+  <si>
+    <t>plate33</t>
+  </si>
+  <si>
+    <t>plate35</t>
+  </si>
+  <si>
+    <t>plate37</t>
+  </si>
+  <si>
+    <t>plate40</t>
+  </si>
+  <si>
+    <t>plate42</t>
+  </si>
+  <si>
+    <t>plate41</t>
+  </si>
+  <si>
+    <t>plate43</t>
+  </si>
+  <si>
+    <t>plate44</t>
+  </si>
+  <si>
+    <t>plate45</t>
+  </si>
+  <si>
+    <t>plate47</t>
+  </si>
+  <si>
+    <t>plate29</t>
+  </si>
+  <si>
+    <t>plate39</t>
   </si>
 </sst>
 </file>
@@ -515,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62FB5B1-B63A-D349-8AF5-6EF81CABB6B8}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1313,6 +1349,258 @@
         <v>10.7</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>20250702</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>20250702</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>20250702</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>20250702</v>
+      </c>
+      <c r="B60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>20250702</v>
+      </c>
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>20250702</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>20250702</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>20250702</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>20250702</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>20250702</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>20250702</v>
+      </c>
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>20250702</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>20250702</v>
+      </c>
+      <c r="B69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>20250702</v>
+      </c>
+      <c r="B70" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>20250702</v>
+      </c>
+      <c r="B71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>20250702</v>
+      </c>
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>20250702</v>
+      </c>
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>20250702</v>
+      </c>
+      <c r="B74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>33.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>